<commit_message>
send logs on email body
</commit_message>
<xml_diff>
--- a/intersect_backtest.xlsx
+++ b/intersect_backtest.xlsx
@@ -482,11 +482,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -792,7 +791,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +804,7 @@
       <c r="A1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -880,7 +879,7 @@
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">

</xml_diff>